<commit_message>
update file paths in bacteria metadata from Cdiphtheriae to bacteria
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594FD5BB-1E30-4683-9BF5-6EB07A15CAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D29C29-7B6F-4DA7-B8AD-63B5B33A23D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -242,24 +242,6 @@
     <t>fasta_path</t>
   </si>
   <si>
-    <t>assets/sample_fastas/Cdiphtheriae/CP040557.fasta</t>
-  </si>
-  <si>
-    <t>assets/sample_fastas/Cdiphtheriae/BX248355.fasta</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/Cdiphtheriae/CP040557_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/Cdiphtheriae/CP040557_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R2.fastq.gz</t>
-  </si>
-  <si>
     <t>BX248355</t>
   </si>
   <si>
@@ -287,16 +269,34 @@
     <t>gff_path</t>
   </si>
   <si>
-    <t>assets/sample_annotations/Cdiphtheriae/CP040557.gff3</t>
-  </si>
-  <si>
-    <t>assets/sample_annotations/Cdiphtheriae/BX248355.gff3</t>
-  </si>
-  <si>
     <t>host_sex</t>
   </si>
   <si>
     <t>host_age</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/bacteria/CP040557.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/bacteria/CP040557.gff3</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/bacteria/CP040557_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/bacteria/CP040557_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/bacteria/BX248355.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/bacteria/BX248355.gff3</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/bacteria/BX248355_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/bacteria/BX248355_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -858,13 +858,13 @@
         <v>47</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>54</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>48</v>
@@ -921,16 +921,16 @@
         <v>15</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="AD2" s="4" t="s">
         <v>16</v>
@@ -951,7 +951,7 @@
         <v>67</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AK2" s="6" t="s">
         <v>21</v>
@@ -1026,13 +1026,13 @@
         <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>60</v>
@@ -1085,10 +1085,10 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>64</v>
@@ -1103,10 +1103,10 @@
         <v>65</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
@@ -1122,22 +1122,22 @@
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>60</v>
@@ -1152,7 +1152,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>63</v>
@@ -1190,13 +1190,13 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="AJ4" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
@@ -1208,10 +1208,10 @@
         <v>65</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>

</xml_diff>

<commit_message>
remove duplicate description col in bacteria metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D29C29-7B6F-4DA7-B8AD-63B5B33A23D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43067090-30B4-46FD-9FA8-7FDCE9020947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
   <si>
     <t>Submission info</t>
   </si>
@@ -758,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:BE45"/>
+  <dimension ref="A1:BD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,10 +769,10 @@
     <col min="1" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" customWidth="1"/>
     <col min="6" max="6" width="23.453125" customWidth="1"/>
-    <col min="7" max="52" width="24" customWidth="1"/>
+    <col min="7" max="51" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -802,26 +802,26 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
+      <c r="AJ1" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="AK1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -829,10 +829,10 @@
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
@@ -842,9 +842,8 @@
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-    </row>
-    <row r="2" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -887,135 +886,132 @@
       <c r="N2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>54</v>
+      <c r="O2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y2" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="Y2" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="Z2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>77</v>
       </c>
+      <c r="AB2" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="AC2" s="4" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="AF2" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="AG2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH2" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="AH2" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="AI2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="AJ2" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="AK2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL2" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="AL2" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="AM2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="AU2" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="AV2" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BA2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BB2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="BC2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="BE2" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1053,27 +1049,27 @@
         <v>63</v>
       </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="Q3" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1" t="s">
+      <c r="V3" s="1"/>
+      <c r="W3" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -1083,31 +1079,31 @@
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
+      <c r="AH3" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="AI3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK3" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
+      <c r="AQ3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AR3" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT3" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
@@ -1118,9 +1114,8 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -1158,27 +1153,27 @@
         <v>63</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="Q4" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1" t="s">
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1" t="s">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -1188,31 +1183,31 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="AH4" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="AI4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK4" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
+      <c r="AQ4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AR4" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AT4" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -1223,30 +1218,29 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
-      <c r="BE4" s="1"/>
-    </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add sequencing data to the metadata file
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43067090-30B4-46FD-9FA8-7FDCE9020947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D62C6-13FD-4019-8151-6A2A43518F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="3420" yWindow="735" windowWidth="25455" windowHeight="20865" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
   <si>
     <t>Submission info</t>
   </si>
@@ -297,6 +297,21 @@
   </si>
   <si>
     <t>assets/sample_fastqs/bacteria/BX248355_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>Illumina MiSeq</t>
+  </si>
+  <si>
+    <t>WGS</t>
+  </si>
+  <si>
+    <t>GENOMIC</t>
+  </si>
+  <si>
+    <t>RANDOM</t>
+  </si>
+  <si>
+    <t>PAIRED</t>
   </si>
 </sst>
 </file>
@@ -462,9 +477,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +517,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -608,7 +623,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,7 +765,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -760,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:BD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1088,11 +1103,21 @@
       <c r="AJ3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
+      <c r="AK3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1" t="s">
         <v>65</v>
@@ -1192,11 +1217,21 @@
       <c r="AJ4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
update metadata templates to add illumina_library_name and nanopore_library_name
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D62C6-13FD-4019-8151-6A2A43518F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0813334C-57D3-42A5-B186-FFC93FBF78E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="735" windowWidth="25455" windowHeight="20865" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>Submission info</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>PAIRED</t>
+  </si>
+  <si>
+    <t>illumina_library_name</t>
+  </si>
+  <si>
+    <t>nanopore_library_name</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,6 +462,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:BD45"/>
+  <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,10 +793,10 @@
     <col min="1" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" customWidth="1"/>
     <col min="6" max="6" width="23.453125" customWidth="1"/>
-    <col min="7" max="51" width="24" customWidth="1"/>
+    <col min="7" max="52" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,10 +853,10 @@
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
@@ -857,8 +866,9 @@
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-    </row>
-    <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BE1" s="1"/>
+    </row>
+    <row r="2" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -986,47 +996,52 @@
         <v>27</v>
       </c>
       <c r="AQ2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BC2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1119,16 +1134,16 @@
         <v>91</v>
       </c>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
@@ -1139,8 +1154,9 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE3" s="1"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -1233,16 +1249,16 @@
         <v>91</v>
       </c>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1" t="s">
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -1253,29 +1269,30 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE4" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add illumina_library_name and nanopore_library_name columns to metadata templates
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D62C6-13FD-4019-8151-6A2A43518F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7FE1AD-76BF-4A1D-B939-C34F9B1B5ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="735" windowWidth="25455" windowHeight="20865" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>Submission info</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>PAIRED</t>
+  </si>
+  <si>
+    <t>illumina_library_name</t>
+  </si>
+  <si>
+    <t>nanopore_library_name</t>
   </si>
 </sst>
 </file>
@@ -773,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:BD45"/>
+  <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BA7" sqref="BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,10 +790,10 @@
     <col min="1" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" customWidth="1"/>
     <col min="6" max="6" width="23.453125" customWidth="1"/>
-    <col min="7" max="51" width="24" customWidth="1"/>
+    <col min="7" max="53" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,10 +850,10 @@
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
@@ -857,8 +863,9 @@
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-    </row>
-    <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BE1" s="1"/>
+    </row>
+    <row r="2" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -986,47 +993,52 @@
         <v>27</v>
       </c>
       <c r="AQ2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1119,16 +1131,16 @@
         <v>91</v>
       </c>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
@@ -1139,8 +1151,9 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE3" s="1"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -1233,16 +1246,16 @@
         <v>91</v>
       </c>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1" t="s">
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -1253,29 +1266,30 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE4" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
illumina_library_name needs a default Not Provided value
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7FE1AD-76BF-4A1D-B939-C34F9B1B5ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B4850F-F0C0-4E0C-BBE9-54F03D588C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="4560" yWindow="4560" windowWidth="28800" windowHeight="12760" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t>Submission info</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>nanopore_library_name</t>
+  </si>
+  <si>
+    <t>Not Provided</t>
   </si>
 </sst>
 </file>
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BA7" sqref="BA7"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,7 +1134,9 @@
         <v>91</v>
       </c>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
+      <c r="AQ3" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="AR3" s="1" t="s">
         <v>65</v>
       </c>
@@ -1246,7 +1251,9 @@
         <v>91</v>
       </c>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
+      <c r="AQ4" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="AR4" s="1" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
change ncbi_sequence_name_sra to ncbi-spuid-sra and update ww template
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/bacteria_test_metadata.xlsx
+++ b/assets/sample_metadata/bacteria_test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FE29F6-2B4B-4855-B51A-8373E2411507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60D03A2-646E-4956-8C26-FEB9A8E263AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3400" windowWidth="28800" windowHeight="12760" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="20790" windowHeight="17800" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>Submission info</t>
   </si>
@@ -101,9 +101,6 @@
     <t>mean_coverage</t>
   </si>
   <si>
-    <t>ncbi_sequence_name_sra</t>
-  </si>
-  <si>
     <t>illumina_sequencing_instrument</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>Cdiphtheriae</t>
   </si>
   <si>
-    <t>SRA - all</t>
-  </si>
-  <si>
     <t>SRA - Illumina info</t>
   </si>
   <si>
@@ -315,6 +309,12 @@
   </si>
   <si>
     <t>Not Provided</t>
+  </si>
+  <si>
+    <t>ncbi-spuid-sra</t>
+  </si>
+  <si>
+    <t>BX248355_Cd</t>
   </si>
 </sst>
 </file>
@@ -779,15 +779,15 @@
   <dimension ref="A1:BD45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="52" width="24" customWidth="1"/>
+    <col min="1" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" customWidth="1"/>
+    <col min="7" max="52" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -795,19 +795,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="3"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -819,24 +819,22 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-      <c r="AI1" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="AI1" s="1"/>
       <c r="AJ1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
@@ -848,7 +846,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -866,227 +864,229 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="J2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="BB2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AR2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AW2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AY2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="BC2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
@@ -1096,42 +1096,40 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="AG3" s="1"/>
       <c r="AH3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="AJ3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AQ3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
@@ -1147,60 +1145,62 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -1210,42 +1210,40 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
-      <c r="AG4" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="AG4" s="1"/>
       <c r="AH4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="AJ4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
@@ -1260,115 +1258,115 @@
       <c r="BD4" s="1"/>
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E45" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F45" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>